<commit_message>
finished creating the SDQ. CBCL & swan diagnosis functions. Fixed some bugs and organized the code
</commit_message>
<xml_diff>
--- a/Irit/data/ADHD.xlsx
+++ b/Irit/data/ADHD.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nogur\Documents\DeppClinic\Irit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32305AC8-200A-49C0-9A3E-F1D1E2A245C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F34BD5A-6393-48E0-8480-4A450E582AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A8B8D4BB-6F3C-472B-AA77-A32C266C2B3A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A8B8D4BB-6F3C-472B-AA77-A32C266C2B3A}"/>
   </bookViews>
   <sheets>
     <sheet name="t1" sheetId="2" r:id="rId1"/>
     <sheet name="גיליון1" sheetId="3" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'t1'!$A$1:$AZ$185</definedName>
   </definedNames>
@@ -38,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="124">
   <si>
     <t>male</t>
   </si>
@@ -416,6 +413,9 @@
   <si>
     <t>נכון מאוד או נכון לעיתים קרובות - very or often true</t>
   </si>
+  <si>
+    <t>gender</t>
+  </si>
 </sst>
 </file>
 
@@ -425,7 +425,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -466,7 +466,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1135,7 +1135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1308,36 +1308,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1348,14 +1323,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1370,29 +1343,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1400,25 +1355,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1433,14 +1373,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1453,29 +1389,89 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1492,27 +1488,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="מקרא - שאלון הורים ודיאגנוסטי"/>
-      <sheetName val="מקרא - שאלון מורה"/>
-      <sheetName val="מקרא - שאלון ילד"/>
-      <sheetName val=" מקרא שאלון אם"/>
-      <sheetName val="מקרא שאלון אב"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1818,16 +1793,16 @@
   </sheetPr>
   <dimension ref="A1:AZ216"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" style="6" customWidth="1"/>
     <col min="2" max="2" width="4" style="28" customWidth="1"/>
     <col min="3" max="8" width="4" style="27" customWidth="1"/>
     <col min="9" max="9" width="4" style="59" customWidth="1"/>
@@ -1841,20 +1816,20 @@
     <col min="26" max="28" width="4" style="59" customWidth="1"/>
     <col min="29" max="29" width="4" style="51" customWidth="1"/>
     <col min="30" max="34" width="4" style="6" customWidth="1"/>
-    <col min="35" max="35" width="5.875" style="21" customWidth="1"/>
-    <col min="36" max="36" width="5.875" style="22" customWidth="1"/>
+    <col min="35" max="35" width="5.90625" style="21" customWidth="1"/>
+    <col min="36" max="36" width="5.90625" style="22" customWidth="1"/>
     <col min="37" max="46" width="4" style="6" customWidth="1"/>
-    <col min="47" max="48" width="5.875" style="6" customWidth="1"/>
+    <col min="47" max="48" width="5.90625" style="6" customWidth="1"/>
     <col min="49" max="52" width="4" style="6" customWidth="1"/>
-    <col min="53" max="16384" width="14.375" style="6"/>
+    <col min="53" max="16384" width="14.36328125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="23" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" s="23" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>3</v>
@@ -2007,7 +1982,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2155,7 +2130,7 @@
       <c r="AY2" s="7"/>
       <c r="AZ2" s="8"/>
     </row>
-    <row r="3" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2303,7 +2278,7 @@
       <c r="AY3" s="7"/>
       <c r="AZ3" s="8"/>
     </row>
-    <row r="4" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2451,7 +2426,7 @@
       <c r="AY4" s="7"/>
       <c r="AZ4" s="8"/>
     </row>
-    <row r="5" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2557,7 +2532,7 @@
       <c r="AY5" s="7"/>
       <c r="AZ5" s="8"/>
     </row>
-    <row r="6" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2705,7 +2680,7 @@
       <c r="AY6" s="7"/>
       <c r="AZ6" s="8"/>
     </row>
-    <row r="7" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2853,7 +2828,7 @@
       <c r="AY7" s="7"/>
       <c r="AZ7" s="8"/>
     </row>
-    <row r="8" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3001,7 +2976,7 @@
       <c r="AY8" s="7"/>
       <c r="AZ8" s="8"/>
     </row>
-    <row r="9" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3149,7 +3124,7 @@
       <c r="AY9" s="7"/>
       <c r="AZ9" s="8"/>
     </row>
-    <row r="10" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3297,7 +3272,7 @@
       <c r="AY10" s="7"/>
       <c r="AZ10" s="8"/>
     </row>
-    <row r="11" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3445,7 +3420,7 @@
       <c r="AY11" s="7"/>
       <c r="AZ11" s="8"/>
     </row>
-    <row r="12" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3593,7 +3568,7 @@
       <c r="AY12" s="7"/>
       <c r="AZ12" s="8"/>
     </row>
-    <row r="13" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3739,7 +3714,7 @@
       <c r="AY13" s="7"/>
       <c r="AZ13" s="8"/>
     </row>
-    <row r="14" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3887,7 +3862,7 @@
       <c r="AY14" s="7"/>
       <c r="AZ14" s="8"/>
     </row>
-    <row r="15" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4035,7 +4010,7 @@
       <c r="AY15" s="7"/>
       <c r="AZ15" s="8"/>
     </row>
-    <row r="16" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4183,7 +4158,7 @@
       <c r="AY16" s="7"/>
       <c r="AZ16" s="8"/>
     </row>
-    <row r="17" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4329,7 +4304,7 @@
       <c r="AY17" s="7"/>
       <c r="AZ17" s="8"/>
     </row>
-    <row r="18" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4477,7 +4452,7 @@
       <c r="AY18" s="7"/>
       <c r="AZ18" s="8"/>
     </row>
-    <row r="19" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4625,7 +4600,7 @@
       <c r="AY19" s="7"/>
       <c r="AZ19" s="8"/>
     </row>
-    <row r="20" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4773,7 +4748,7 @@
       <c r="AY20" s="7"/>
       <c r="AZ20" s="8"/>
     </row>
-    <row r="21" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4921,7 +4896,7 @@
       <c r="AY21" s="7"/>
       <c r="AZ21" s="8"/>
     </row>
-    <row r="22" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5067,7 +5042,7 @@
       <c r="AY22" s="7"/>
       <c r="AZ22" s="8"/>
     </row>
-    <row r="23" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5215,7 +5190,7 @@
       <c r="AY23" s="7"/>
       <c r="AZ23" s="8"/>
     </row>
-    <row r="24" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5363,7 +5338,7 @@
       <c r="AY24" s="7"/>
       <c r="AZ24" s="8"/>
     </row>
-    <row r="25" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5511,7 +5486,7 @@
       <c r="AY25" s="7"/>
       <c r="AZ25" s="8"/>
     </row>
-    <row r="26" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5659,7 +5634,7 @@
       <c r="AY26" s="7"/>
       <c r="AZ26" s="8"/>
     </row>
-    <row r="27" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5807,7 +5782,7 @@
       <c r="AY27" s="7"/>
       <c r="AZ27" s="8"/>
     </row>
-    <row r="28" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5955,7 +5930,7 @@
       <c r="AY28" s="7"/>
       <c r="AZ28" s="8"/>
     </row>
-    <row r="29" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -6103,7 +6078,7 @@
       <c r="AY29" s="7"/>
       <c r="AZ29" s="8"/>
     </row>
-    <row r="30" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -6251,7 +6226,7 @@
       <c r="AY30" s="7"/>
       <c r="AZ30" s="8"/>
     </row>
-    <row r="31" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -6399,7 +6374,7 @@
       <c r="AY31" s="7"/>
       <c r="AZ31" s="8"/>
     </row>
-    <row r="32" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -6547,7 +6522,7 @@
       <c r="AY32" s="7"/>
       <c r="AZ32" s="8"/>
     </row>
-    <row r="33" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -6695,7 +6670,7 @@
       <c r="AY33" s="7"/>
       <c r="AZ33" s="8"/>
     </row>
-    <row r="34" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -6843,7 +6818,7 @@
       <c r="AY34" s="7"/>
       <c r="AZ34" s="8"/>
     </row>
-    <row r="35" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -6991,7 +6966,7 @@
       <c r="AY35" s="7"/>
       <c r="AZ35" s="8"/>
     </row>
-    <row r="36" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -7139,7 +7114,7 @@
       <c r="AY36" s="7"/>
       <c r="AZ36" s="8"/>
     </row>
-    <row r="37" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -7287,7 +7262,7 @@
       <c r="AY37" s="7"/>
       <c r="AZ37" s="8"/>
     </row>
-    <row r="38" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -7435,7 +7410,7 @@
       <c r="AY38" s="7"/>
       <c r="AZ38" s="8"/>
     </row>
-    <row r="39" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -7583,7 +7558,7 @@
       <c r="AY39" s="7"/>
       <c r="AZ39" s="8"/>
     </row>
-    <row r="40" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -7731,7 +7706,7 @@
       <c r="AY40" s="7"/>
       <c r="AZ40" s="8"/>
     </row>
-    <row r="41" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -7877,7 +7852,7 @@
       <c r="AY41" s="7"/>
       <c r="AZ41" s="8"/>
     </row>
-    <row r="42" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -8025,7 +8000,7 @@
       <c r="AY42" s="7"/>
       <c r="AZ42" s="8"/>
     </row>
-    <row r="43" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -8173,7 +8148,7 @@
       <c r="AY43" s="7"/>
       <c r="AZ43" s="8"/>
     </row>
-    <row r="44" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -8321,7 +8296,7 @@
       <c r="AY44" s="7"/>
       <c r="AZ44" s="8"/>
     </row>
-    <row r="45" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -8469,7 +8444,7 @@
       <c r="AY45" s="7"/>
       <c r="AZ45" s="8"/>
     </row>
-    <row r="46" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -8617,7 +8592,7 @@
       <c r="AY46" s="7"/>
       <c r="AZ46" s="8"/>
     </row>
-    <row r="47" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -8765,7 +8740,7 @@
       <c r="AY47" s="7"/>
       <c r="AZ47" s="8"/>
     </row>
-    <row r="48" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -8913,7 +8888,7 @@
       <c r="AY48" s="7"/>
       <c r="AZ48" s="8"/>
     </row>
-    <row r="49" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -9059,7 +9034,7 @@
       <c r="AY49" s="7"/>
       <c r="AZ49" s="8"/>
     </row>
-    <row r="50" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -9207,7 +9182,7 @@
       <c r="AY50" s="7"/>
       <c r="AZ50" s="8"/>
     </row>
-    <row r="51" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -9355,7 +9330,7 @@
       <c r="AY51" s="7"/>
       <c r="AZ51" s="8"/>
     </row>
-    <row r="52" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -9503,7 +9478,7 @@
       <c r="AY52" s="7"/>
       <c r="AZ52" s="8"/>
     </row>
-    <row r="53" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -9651,7 +9626,7 @@
       <c r="AY53" s="7"/>
       <c r="AZ53" s="8"/>
     </row>
-    <row r="54" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -9799,7 +9774,7 @@
       <c r="AY54" s="7"/>
       <c r="AZ54" s="8"/>
     </row>
-    <row r="55" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -9945,7 +9920,7 @@
       <c r="AY55" s="7"/>
       <c r="AZ55" s="8"/>
     </row>
-    <row r="56" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -10093,7 +10068,7 @@
       <c r="AY56" s="7"/>
       <c r="AZ56" s="8"/>
     </row>
-    <row r="57" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -10241,7 +10216,7 @@
       <c r="AY57" s="7"/>
       <c r="AZ57" s="8"/>
     </row>
-    <row r="58" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -10389,7 +10364,7 @@
       <c r="AY58" s="7"/>
       <c r="AZ58" s="8"/>
     </row>
-    <row r="59" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -10451,7 +10426,7 @@
       <c r="AY59" s="7"/>
       <c r="AZ59" s="8"/>
     </row>
-    <row r="60" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -10599,7 +10574,7 @@
       <c r="AY60" s="7"/>
       <c r="AZ60" s="8"/>
     </row>
-    <row r="61" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -10745,7 +10720,7 @@
       <c r="AY61" s="7"/>
       <c r="AZ61" s="8"/>
     </row>
-    <row r="62" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -10893,7 +10868,7 @@
       <c r="AY62" s="7"/>
       <c r="AZ62" s="8"/>
     </row>
-    <row r="63" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -11003,7 +10978,7 @@
       <c r="AY63" s="7"/>
       <c r="AZ63" s="8"/>
     </row>
-    <row r="64" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -11151,7 +11126,7 @@
       <c r="AY64" s="7"/>
       <c r="AZ64" s="8"/>
     </row>
-    <row r="65" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -11299,7 +11274,7 @@
       <c r="AY65" s="7"/>
       <c r="AZ65" s="8"/>
     </row>
-    <row r="66" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -11447,7 +11422,7 @@
       <c r="AY66" s="7"/>
       <c r="AZ66" s="8"/>
     </row>
-    <row r="67" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -11595,7 +11570,7 @@
       <c r="AY67" s="7"/>
       <c r="AZ67" s="8"/>
     </row>
-    <row r="68" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -11657,7 +11632,7 @@
       <c r="AY68" s="7"/>
       <c r="AZ68" s="8"/>
     </row>
-    <row r="69" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -11803,7 +11778,7 @@
       <c r="AY69" s="7"/>
       <c r="AZ69" s="8"/>
     </row>
-    <row r="70" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -11951,7 +11926,7 @@
       <c r="AY70" s="7"/>
       <c r="AZ70" s="8"/>
     </row>
-    <row r="71" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -12099,7 +12074,7 @@
       <c r="AY71" s="7"/>
       <c r="AZ71" s="8"/>
     </row>
-    <row r="72" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -12247,7 +12222,7 @@
       <c r="AY72" s="7"/>
       <c r="AZ72" s="8"/>
     </row>
-    <row r="73" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -12395,7 +12370,7 @@
       <c r="AY73" s="7"/>
       <c r="AZ73" s="8"/>
     </row>
-    <row r="74" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -12543,7 +12518,7 @@
       <c r="AY74" s="7"/>
       <c r="AZ74" s="8"/>
     </row>
-    <row r="75" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -12691,7 +12666,7 @@
       <c r="AY75" s="7"/>
       <c r="AZ75" s="8"/>
     </row>
-    <row r="76" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -12839,7 +12814,7 @@
       <c r="AY76" s="7"/>
       <c r="AZ76" s="8"/>
     </row>
-    <row r="77" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -12983,7 +12958,7 @@
       <c r="AY77" s="7"/>
       <c r="AZ77" s="8"/>
     </row>
-    <row r="78" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -13131,7 +13106,7 @@
       <c r="AY78" s="7"/>
       <c r="AZ78" s="8"/>
     </row>
-    <row r="79" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -13277,7 +13252,7 @@
       <c r="AY79" s="7"/>
       <c r="AZ79" s="8"/>
     </row>
-    <row r="80" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -13425,7 +13400,7 @@
       <c r="AY80" s="7"/>
       <c r="AZ80" s="8"/>
     </row>
-    <row r="81" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -13573,7 +13548,7 @@
       <c r="AY81" s="7"/>
       <c r="AZ81" s="8"/>
     </row>
-    <row r="82" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -13719,7 +13694,7 @@
       <c r="AY82" s="7"/>
       <c r="AZ82" s="8"/>
     </row>
-    <row r="83" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -13867,7 +13842,7 @@
       <c r="AY83" s="7"/>
       <c r="AZ83" s="8"/>
     </row>
-    <row r="84" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -14013,7 +13988,7 @@
       <c r="AY84" s="7"/>
       <c r="AZ84" s="8"/>
     </row>
-    <row r="85" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -14159,7 +14134,7 @@
       <c r="AY85" s="7"/>
       <c r="AZ85" s="8"/>
     </row>
-    <row r="86" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -14307,7 +14282,7 @@
       <c r="AY86" s="7"/>
       <c r="AZ86" s="8"/>
     </row>
-    <row r="87" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -14447,7 +14422,7 @@
       <c r="AY87" s="7"/>
       <c r="AZ87" s="8"/>
     </row>
-    <row r="88" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -14595,7 +14570,7 @@
       <c r="AY88" s="7"/>
       <c r="AZ88" s="8"/>
     </row>
-    <row r="89" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -14743,7 +14718,7 @@
       <c r="AY89" s="7"/>
       <c r="AZ89" s="8"/>
     </row>
-    <row r="90" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -14891,7 +14866,7 @@
       <c r="AY90" s="7"/>
       <c r="AZ90" s="8"/>
     </row>
-    <row r="91" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -15039,7 +15014,7 @@
       <c r="AY91" s="7"/>
       <c r="AZ91" s="8"/>
     </row>
-    <row r="92" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -15101,7 +15076,7 @@
       <c r="AY92" s="7"/>
       <c r="AZ92" s="8"/>
     </row>
-    <row r="93" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -15249,7 +15224,7 @@
       <c r="AY93" s="7"/>
       <c r="AZ93" s="8"/>
     </row>
-    <row r="94" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -15397,7 +15372,7 @@
       <c r="AY94" s="7"/>
       <c r="AZ94" s="8"/>
     </row>
-    <row r="95" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -15545,7 +15520,7 @@
       <c r="AY95" s="7"/>
       <c r="AZ95" s="8"/>
     </row>
-    <row r="96" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -15693,7 +15668,7 @@
       <c r="AY96" s="7"/>
       <c r="AZ96" s="8"/>
     </row>
-    <row r="97" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -15841,7 +15816,7 @@
       <c r="AY97" s="7"/>
       <c r="AZ97" s="8"/>
     </row>
-    <row r="98" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -15945,7 +15920,7 @@
       <c r="AY98" s="7"/>
       <c r="AZ98" s="8"/>
     </row>
-    <row r="99" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -16089,7 +16064,7 @@
       <c r="AY99" s="7"/>
       <c r="AZ99" s="8"/>
     </row>
-    <row r="100" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -16237,7 +16212,7 @@
       <c r="AY100" s="7"/>
       <c r="AZ100" s="8"/>
     </row>
-    <row r="101" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -16385,7 +16360,7 @@
       <c r="AY101" s="7"/>
       <c r="AZ101" s="8"/>
     </row>
-    <row r="102" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -16533,7 +16508,7 @@
       <c r="AY102" s="7"/>
       <c r="AZ102" s="8"/>
     </row>
-    <row r="103" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -16681,7 +16656,7 @@
       <c r="AY103" s="7"/>
       <c r="AZ103" s="8"/>
     </row>
-    <row r="104" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -16829,7 +16804,7 @@
       <c r="AY104" s="7"/>
       <c r="AZ104" s="8"/>
     </row>
-    <row r="105" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -16935,7 +16910,7 @@
       <c r="AY105" s="7"/>
       <c r="AZ105" s="8"/>
     </row>
-    <row r="106" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -17079,7 +17054,7 @@
       <c r="AY106" s="7"/>
       <c r="AZ106" s="8"/>
     </row>
-    <row r="107" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -17227,7 +17202,7 @@
       <c r="AY107" s="7"/>
       <c r="AZ107" s="8"/>
     </row>
-    <row r="108" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -17289,7 +17264,7 @@
       <c r="AY108" s="7"/>
       <c r="AZ108" s="8"/>
     </row>
-    <row r="109" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -17437,7 +17412,7 @@
       <c r="AY109" s="7"/>
       <c r="AZ109" s="8"/>
     </row>
-    <row r="110" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -17585,7 +17560,7 @@
       <c r="AY110" s="7"/>
       <c r="AZ110" s="8"/>
     </row>
-    <row r="111" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -17647,7 +17622,7 @@
       <c r="AY111" s="7"/>
       <c r="AZ111" s="8"/>
     </row>
-    <row r="112" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -17795,7 +17770,7 @@
       <c r="AY112" s="7"/>
       <c r="AZ112" s="8"/>
     </row>
-    <row r="113" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -17943,7 +17918,7 @@
       <c r="AY113" s="7"/>
       <c r="AZ113" s="8"/>
     </row>
-    <row r="114" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -18091,7 +18066,7 @@
       <c r="AY114" s="7"/>
       <c r="AZ114" s="8"/>
     </row>
-    <row r="115" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -18239,7 +18214,7 @@
       <c r="AY115" s="7"/>
       <c r="AZ115" s="8"/>
     </row>
-    <row r="116" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -18301,7 +18276,7 @@
       <c r="AY116" s="7"/>
       <c r="AZ116" s="8"/>
     </row>
-    <row r="117" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -18449,7 +18424,7 @@
       <c r="AY117" s="7"/>
       <c r="AZ117" s="8"/>
     </row>
-    <row r="118" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -18597,7 +18572,7 @@
       <c r="AY118" s="7"/>
       <c r="AZ118" s="8"/>
     </row>
-    <row r="119" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -18745,7 +18720,7 @@
       <c r="AY119" s="7"/>
       <c r="AZ119" s="8"/>
     </row>
-    <row r="120" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -18893,7 +18868,7 @@
       <c r="AY120" s="7"/>
       <c r="AZ120" s="8"/>
     </row>
-    <row r="121" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -19041,7 +19016,7 @@
       <c r="AY121" s="7"/>
       <c r="AZ121" s="8"/>
     </row>
-    <row r="122" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -19189,7 +19164,7 @@
       <c r="AY122" s="7"/>
       <c r="AZ122" s="8"/>
     </row>
-    <row r="123" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -19337,7 +19312,7 @@
       <c r="AY123" s="7"/>
       <c r="AZ123" s="8"/>
     </row>
-    <row r="124" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -19485,7 +19460,7 @@
       <c r="AY124" s="7"/>
       <c r="AZ124" s="8"/>
     </row>
-    <row r="125" spans="1:52" s="18" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:52" s="18" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="33">
         <v>124</v>
       </c>
@@ -19591,7 +19566,7 @@
       <c r="AY125" s="7"/>
       <c r="AZ125" s="8"/>
     </row>
-    <row r="126" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -19695,7 +19670,7 @@
       <c r="AY126" s="7"/>
       <c r="AZ126" s="8"/>
     </row>
-    <row r="127" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -19843,7 +19818,7 @@
       <c r="AY127" s="7"/>
       <c r="AZ127" s="8"/>
     </row>
-    <row r="128" spans="1:52" s="19" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:52" s="19" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="34">
         <v>127</v>
       </c>
@@ -19991,7 +19966,7 @@
       <c r="AY128" s="7"/>
       <c r="AZ128" s="8"/>
     </row>
-    <row r="129" spans="1:52" s="19" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:52" s="19" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="34">
         <v>128</v>
       </c>
@@ -20053,7 +20028,7 @@
       <c r="AY129" s="7"/>
       <c r="AZ129" s="8"/>
     </row>
-    <row r="130" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -20201,7 +20176,7 @@
       <c r="AY130" s="7"/>
       <c r="AZ130" s="8"/>
     </row>
-    <row r="131" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -20263,7 +20238,7 @@
       <c r="AY131" s="7"/>
       <c r="AZ131" s="8"/>
     </row>
-    <row r="132" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -20373,7 +20348,7 @@
       <c r="AY132" s="7"/>
       <c r="AZ132" s="8"/>
     </row>
-    <row r="133" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -20521,7 +20496,7 @@
       <c r="AY133" s="7"/>
       <c r="AZ133" s="8"/>
     </row>
-    <row r="134" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -20669,7 +20644,7 @@
       <c r="AY134" s="7"/>
       <c r="AZ134" s="8"/>
     </row>
-    <row r="135" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -20817,7 +20792,7 @@
       <c r="AY135" s="7"/>
       <c r="AZ135" s="8"/>
     </row>
-    <row r="136" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -20879,7 +20854,7 @@
       <c r="AY136" s="7"/>
       <c r="AZ136" s="8"/>
     </row>
-    <row r="137" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -21019,7 +20994,7 @@
       <c r="AY137" s="7"/>
       <c r="AZ137" s="8"/>
     </row>
-    <row r="138" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -21167,7 +21142,7 @@
       <c r="AY138" s="7"/>
       <c r="AZ138" s="8"/>
     </row>
-    <row r="139" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -21315,7 +21290,7 @@
       <c r="AY139" s="7"/>
       <c r="AZ139" s="8"/>
     </row>
-    <row r="140" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -21463,7 +21438,7 @@
       <c r="AY140" s="7"/>
       <c r="AZ140" s="8"/>
     </row>
-    <row r="141" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -21525,7 +21500,7 @@
       <c r="AY141" s="7"/>
       <c r="AZ141" s="8"/>
     </row>
-    <row r="142" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -21629,7 +21604,7 @@
       <c r="AY142" s="7"/>
       <c r="AZ142" s="8"/>
     </row>
-    <row r="143" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -21777,7 +21752,7 @@
       <c r="AY143" s="7"/>
       <c r="AZ143" s="8"/>
     </row>
-    <row r="144" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -21921,7 +21896,7 @@
       <c r="AY144" s="7"/>
       <c r="AZ144" s="8"/>
     </row>
-    <row r="145" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -22065,7 +22040,7 @@
       <c r="AY145" s="7"/>
       <c r="AZ145" s="8"/>
     </row>
-    <row r="146" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -22213,7 +22188,7 @@
       <c r="AY146" s="7"/>
       <c r="AZ146" s="8"/>
     </row>
-    <row r="147" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -22361,7 +22336,7 @@
       <c r="AY147" s="7"/>
       <c r="AZ147" s="8"/>
     </row>
-    <row r="148" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -22509,7 +22484,7 @@
       <c r="AY148" s="7"/>
       <c r="AZ148" s="8"/>
     </row>
-    <row r="149" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -22657,7 +22632,7 @@
       <c r="AY149" s="7"/>
       <c r="AZ149" s="8"/>
     </row>
-    <row r="150" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -22719,7 +22694,7 @@
       <c r="AY150" s="7"/>
       <c r="AZ150" s="8"/>
     </row>
-    <row r="151" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -22867,7 +22842,7 @@
       <c r="AY151" s="7"/>
       <c r="AZ151" s="8"/>
     </row>
-    <row r="152" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -23015,7 +22990,7 @@
       <c r="AY152" s="7"/>
       <c r="AZ152" s="8"/>
     </row>
-    <row r="153" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -23163,7 +23138,7 @@
       <c r="AY153" s="7"/>
       <c r="AZ153" s="8"/>
     </row>
-    <row r="154" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -23311,7 +23286,7 @@
       <c r="AY154" s="7"/>
       <c r="AZ154" s="8"/>
     </row>
-    <row r="155" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -23459,7 +23434,7 @@
       <c r="AY155" s="7"/>
       <c r="AZ155" s="8"/>
     </row>
-    <row r="156" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -23607,7 +23582,7 @@
       <c r="AY156" s="7"/>
       <c r="AZ156" s="8"/>
     </row>
-    <row r="157" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -23711,7 +23686,7 @@
       <c r="AY157" s="7"/>
       <c r="AZ157" s="8"/>
     </row>
-    <row r="158" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -23859,7 +23834,7 @@
       <c r="AY158" s="7"/>
       <c r="AZ158" s="8"/>
     </row>
-    <row r="159" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -23971,7 +23946,7 @@
       <c r="AY159" s="7"/>
       <c r="AZ159" s="8"/>
     </row>
-    <row r="160" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -24119,7 +24094,7 @@
       <c r="AY160" s="7"/>
       <c r="AZ160" s="8"/>
     </row>
-    <row r="161" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -24267,7 +24242,7 @@
       <c r="AY161" s="7"/>
       <c r="AZ161" s="8"/>
     </row>
-    <row r="162" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -24415,7 +24390,7 @@
       <c r="AY162" s="7"/>
       <c r="AZ162" s="8"/>
     </row>
-    <row r="163" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -24563,7 +24538,7 @@
       <c r="AY163" s="7"/>
       <c r="AZ163" s="8"/>
     </row>
-    <row r="164" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -24711,7 +24686,7 @@
       <c r="AY164" s="7"/>
       <c r="AZ164" s="8"/>
     </row>
-    <row r="165" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -24859,7 +24834,7 @@
       <c r="AY165" s="7"/>
       <c r="AZ165" s="8"/>
     </row>
-    <row r="166" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -25007,7 +24982,7 @@
       <c r="AY166" s="7"/>
       <c r="AZ166" s="8"/>
     </row>
-    <row r="167" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -25155,7 +25130,7 @@
       <c r="AY167" s="7"/>
       <c r="AZ167" s="8"/>
     </row>
-    <row r="168" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -25303,7 +25278,7 @@
       <c r="AY168" s="7"/>
       <c r="AZ168" s="8"/>
     </row>
-    <row r="169" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -25451,7 +25426,7 @@
       <c r="AY169" s="7"/>
       <c r="AZ169" s="8"/>
     </row>
-    <row r="170" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -25599,7 +25574,7 @@
       <c r="AY170" s="7"/>
       <c r="AZ170" s="8"/>
     </row>
-    <row r="171" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -25737,7 +25712,7 @@
       <c r="AY171" s="7"/>
       <c r="AZ171" s="8"/>
     </row>
-    <row r="172" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -25807,7 +25782,7 @@
       <c r="AY172" s="7"/>
       <c r="AZ172" s="8"/>
     </row>
-    <row r="173" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -25869,7 +25844,7 @@
       <c r="AY173" s="7"/>
       <c r="AZ173" s="8"/>
     </row>
-    <row r="174" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -26017,7 +25992,7 @@
       <c r="AY174" s="7"/>
       <c r="AZ174" s="8"/>
     </row>
-    <row r="175" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -26165,7 +26140,7 @@
       <c r="AY175" s="7"/>
       <c r="AZ175" s="8"/>
     </row>
-    <row r="176" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -26313,7 +26288,7 @@
       <c r="AY176" s="7"/>
       <c r="AZ176" s="8"/>
     </row>
-    <row r="177" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -26457,7 +26432,7 @@
       <c r="AY177" s="7"/>
       <c r="AZ177" s="8"/>
     </row>
-    <row r="178" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -26605,7 +26580,7 @@
       <c r="AY178" s="7"/>
       <c r="AZ178" s="8"/>
     </row>
-    <row r="179" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -26753,7 +26728,7 @@
       <c r="AY179" s="7"/>
       <c r="AZ179" s="8"/>
     </row>
-    <row r="180" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -26901,7 +26876,7 @@
       <c r="AY180" s="7"/>
       <c r="AZ180" s="8"/>
     </row>
-    <row r="181" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -27049,7 +27024,7 @@
       <c r="AY181" s="7"/>
       <c r="AZ181" s="8"/>
     </row>
-    <row r="182" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -27111,7 +27086,7 @@
       <c r="AY182" s="7"/>
       <c r="AZ182" s="8"/>
     </row>
-    <row r="183" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -27173,7 +27148,7 @@
       <c r="AY183" s="7"/>
       <c r="AZ183" s="8"/>
     </row>
-    <row r="184" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -27321,7 +27296,7 @@
       <c r="AY184" s="7"/>
       <c r="AZ184" s="8"/>
     </row>
-    <row r="185" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -27469,7 +27444,7 @@
       <c r="AY185" s="7"/>
       <c r="AZ185" s="8"/>
     </row>
-    <row r="186" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E186" s="25"/>
       <c r="F186" s="26"/>
       <c r="G186" s="26"/>
@@ -27477,27 +27452,27 @@
       <c r="AI186" s="6"/>
       <c r="AJ186" s="6"/>
     </row>
-    <row r="187" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI187" s="6"/>
       <c r="AJ187" s="6"/>
     </row>
-    <row r="188" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI188" s="6"/>
       <c r="AJ188" s="6"/>
     </row>
-    <row r="189" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI189" s="6"/>
       <c r="AJ189" s="6"/>
     </row>
-    <row r="190" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI190" s="6"/>
       <c r="AJ190" s="6"/>
     </row>
-    <row r="191" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI191" s="6"/>
       <c r="AJ191" s="6"/>
     </row>
-    <row r="192" spans="1:52" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:52" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="6"/>
       <c r="B192" s="28"/>
       <c r="C192" s="27"/>
@@ -27551,99 +27526,99 @@
       <c r="AY192" s="6"/>
       <c r="AZ192" s="6"/>
     </row>
-    <row r="193" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI193" s="6"/>
       <c r="AJ193" s="6"/>
     </row>
-    <row r="194" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI194" s="6"/>
       <c r="AJ194" s="6"/>
     </row>
-    <row r="195" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI195" s="6"/>
       <c r="AJ195" s="6"/>
     </row>
-    <row r="196" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI196" s="6"/>
       <c r="AJ196" s="6"/>
     </row>
-    <row r="197" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI197" s="6"/>
       <c r="AJ197" s="6"/>
     </row>
-    <row r="198" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI198" s="6"/>
       <c r="AJ198" s="6"/>
     </row>
-    <row r="199" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI199" s="6"/>
       <c r="AJ199" s="6"/>
     </row>
-    <row r="200" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI200" s="6"/>
       <c r="AJ200" s="6"/>
     </row>
-    <row r="201" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI201" s="6"/>
       <c r="AJ201" s="6"/>
     </row>
-    <row r="202" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI202" s="6"/>
       <c r="AJ202" s="6"/>
     </row>
-    <row r="203" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI203" s="6"/>
       <c r="AJ203" s="6"/>
     </row>
-    <row r="204" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI204" s="6"/>
       <c r="AJ204" s="6"/>
     </row>
-    <row r="205" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI205" s="6"/>
       <c r="AJ205" s="6"/>
     </row>
-    <row r="206" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI206" s="6"/>
       <c r="AJ206" s="6"/>
     </row>
-    <row r="207" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI207" s="6"/>
       <c r="AJ207" s="6"/>
     </row>
-    <row r="208" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI208" s="6"/>
       <c r="AJ208" s="6"/>
     </row>
-    <row r="209" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI209" s="6"/>
       <c r="AJ209" s="6"/>
     </row>
-    <row r="210" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI210" s="6"/>
       <c r="AJ210" s="6"/>
     </row>
-    <row r="211" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI211" s="6"/>
       <c r="AJ211" s="6"/>
     </row>
-    <row r="212" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI212" s="6"/>
       <c r="AJ212" s="6"/>
     </row>
-    <row r="213" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI213" s="6"/>
       <c r="AJ213" s="6"/>
     </row>
-    <row r="214" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI214" s="6"/>
       <c r="AJ214" s="6"/>
     </row>
-    <row r="215" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI215" s="6"/>
       <c r="AJ215" s="6"/>
     </row>
-    <row r="216" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="35:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AI216" s="6"/>
       <c r="AJ216" s="6"/>
     </row>
@@ -27658,485 +27633,487 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A74DA0F8-3891-4027-8B5B-60EBB28ED419}">
   <dimension ref="B1:E51"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView rightToLeft="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.875" customWidth="1"/>
-    <col min="2" max="2" width="47.125" customWidth="1"/>
-    <col min="3" max="3" width="31.375" customWidth="1"/>
+    <col min="1" max="1" width="4.90625" customWidth="1"/>
+    <col min="2" max="2" width="47.08984375" customWidth="1"/>
+    <col min="3" max="3" width="31.36328125" customWidth="1"/>
     <col min="4" max="4" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="113" t="s">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="106" t="s">
+      <c r="C2" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="87" t="s">
+      <c r="E2" s="125" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="125">
-        <v>0</v>
-      </c>
-      <c r="C3" s="112" t="s">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="99">
+        <v>0</v>
+      </c>
+      <c r="C3" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="112"/>
-      <c r="E3" s="87"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="125"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="126">
-        <v>1</v>
-      </c>
-      <c r="C4" s="117" t="s">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="100">
+        <v>1</v>
+      </c>
+      <c r="C4" s="104" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="117"/>
-      <c r="E4" s="87"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="125"/>
     </row>
-    <row r="5" spans="2:5" s="111" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="126">
-        <v>2</v>
-      </c>
-      <c r="C5" s="117" t="s">
+    <row r="5" spans="2:5" s="88" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="100">
+        <v>2</v>
+      </c>
+      <c r="C5" s="104" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="117"/>
-      <c r="E5" s="87"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="125"/>
     </row>
-    <row r="6" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="118" t="s">
+    <row r="6" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="93" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="119" t="s">
+      <c r="C6" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="119" t="s">
+      <c r="D6" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="87"/>
+      <c r="E6" s="125"/>
     </row>
-    <row r="7" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="120" t="s">
+    <row r="7" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="119" t="s">
+      <c r="C7" s="94" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="119" t="s">
+      <c r="D7" s="94" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="87"/>
+      <c r="E7" s="125"/>
     </row>
-    <row r="8" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="121" t="s">
+    <row r="8" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="122" t="s">
+      <c r="D8" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="87"/>
+      <c r="E8" s="125"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="121" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="122" t="s">
+      <c r="C9" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="122" t="s">
+      <c r="D9" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="87"/>
+      <c r="E9" s="125"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="121" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="96" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="97" t="s">
         <v>119</v>
       </c>
-      <c r="D10" s="122"/>
-      <c r="E10" s="109"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="76"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="123" t="s">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="98" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="124" t="s">
+      <c r="C11" s="97" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="123"/>
+      <c r="D11" s="98"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="127"/>
-      <c r="C12" s="110"/>
-      <c r="D12" s="127"/>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C12" s="87"/>
     </row>
-    <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="114" t="s">
+    <row r="13" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="90" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="115" t="s">
+      <c r="C13" s="91" t="s">
         <v>114</v>
       </c>
-      <c r="D13" s="116" t="s">
+      <c r="D13" s="92" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B14" s="88" t="s">
+    <row r="14" spans="2:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="B14" s="114" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="116" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="90" t="s">
+      <c r="D14" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="91" t="s">
+      <c r="E14" s="118" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="92"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="94" t="s">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="115"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="95"/>
+      <c r="E15" s="119"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="92"/>
-      <c r="C16" s="93"/>
-      <c r="D16" s="94" t="s">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="115"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="E16" s="95"/>
+      <c r="E16" s="119"/>
     </row>
-    <row r="17" spans="2:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B17" s="92"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="96" t="s">
+    <row r="17" spans="2:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="B17" s="115"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="95"/>
+      <c r="E17" s="119"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="92"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="94" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="115"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="95"/>
+      <c r="E18" s="119"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="92"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="96" t="s">
+    <row r="19" spans="2:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="B19" s="115"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="95"/>
+      <c r="E19" s="119"/>
     </row>
-    <row r="20" spans="2:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B20" s="92"/>
-      <c r="C20" s="93"/>
-      <c r="D20" s="96" t="s">
+    <row r="20" spans="2:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="B20" s="115"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="95"/>
+      <c r="E20" s="119"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="92"/>
-      <c r="C21" s="93"/>
-      <c r="D21" s="94" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="115"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="78" t="s">
         <v>98</v>
       </c>
-      <c r="E21" s="95"/>
+      <c r="E21" s="119"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="92"/>
-      <c r="C22" s="93"/>
-      <c r="D22" s="94" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="115"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="78" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="95"/>
+      <c r="E22" s="119"/>
     </row>
-    <row r="23" spans="2:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B23" s="92"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="96" t="s">
+    <row r="23" spans="2:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="B23" s="115"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="95"/>
+      <c r="E23" s="119"/>
     </row>
-    <row r="24" spans="2:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B24" s="92"/>
-      <c r="C24" s="93"/>
-      <c r="D24" s="96" t="s">
+    <row r="24" spans="2:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="B24" s="115"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="95"/>
+      <c r="E24" s="119"/>
     </row>
-    <row r="25" spans="2:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B25" s="92"/>
-      <c r="C25" s="93"/>
-      <c r="D25" s="96" t="s">
+    <row r="25" spans="2:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="B25" s="115"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="E25" s="95"/>
+      <c r="E25" s="119"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="92"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="96" t="s">
+    <row r="26" spans="2:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="B26" s="115"/>
+      <c r="C26" s="117"/>
+      <c r="D26" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="E26" s="95"/>
+      <c r="E26" s="119"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="92"/>
-      <c r="C27" s="93"/>
-      <c r="D27" s="96" t="s">
+    <row r="27" spans="2:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="B27" s="115"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="E27" s="95"/>
+      <c r="E27" s="119"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="92"/>
-      <c r="C28" s="93"/>
-      <c r="D28" s="96" t="s">
+    <row r="28" spans="2:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="B28" s="115"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="E28" s="95"/>
+      <c r="E28" s="119"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="92"/>
-      <c r="C29" s="93"/>
-      <c r="D29" s="96" t="s">
+    <row r="29" spans="2:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="B29" s="115"/>
+      <c r="C29" s="117"/>
+      <c r="D29" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="95"/>
+      <c r="E29" s="119"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="92"/>
-      <c r="C30" s="93"/>
-      <c r="D30" s="96" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="115"/>
+      <c r="C30" s="117"/>
+      <c r="D30" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="95"/>
+      <c r="E30" s="119"/>
     </row>
-    <row r="31" spans="2:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="92"/>
-      <c r="C31" s="93"/>
-      <c r="D31" s="97" t="s">
+    <row r="31" spans="2:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="115"/>
+      <c r="C31" s="117"/>
+      <c r="D31" s="80" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="95"/>
+      <c r="E31" s="119"/>
     </row>
-    <row r="32" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="98" t="s">
+    <row r="32" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="121" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="99"/>
-      <c r="D32" s="100" t="s">
+      <c r="C32" s="122"/>
+      <c r="D32" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="E32" s="95"/>
+      <c r="E32" s="119"/>
     </row>
-    <row r="33" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="101" t="s">
+    <row r="33" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="123" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="102"/>
-      <c r="D33" s="103" t="s">
+      <c r="C33" s="124"/>
+      <c r="D33" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="104"/>
+      <c r="E33" s="120"/>
     </row>
-    <row r="35" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B36" s="105" t="s">
+    <row r="35" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="106" t="s">
+      <c r="C36" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="107" t="s">
+      <c r="D36" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="E36" s="86"/>
+      <c r="E36" s="75"/>
     </row>
-    <row r="37" spans="2:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B37" s="62">
         <v>1</v>
       </c>
       <c r="C37" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="64" t="s">
+      <c r="D37" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="E37" s="108" t="s">
+      <c r="E37" s="86" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B38" s="65">
-        <v>2</v>
-      </c>
-      <c r="C38" s="66" t="s">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" s="64">
+        <v>2</v>
+      </c>
+      <c r="C38" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="67"/>
-      <c r="E38" s="86"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="75"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="68" t="s">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B39" s="107" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="69"/>
-      <c r="D39" s="70" t="s">
+      <c r="C39" s="108"/>
+      <c r="D39" s="111" t="s">
         <v>73</v>
       </c>
-      <c r="E39" s="86"/>
+      <c r="E39" s="75"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="71"/>
-      <c r="C40" s="72"/>
-      <c r="D40" s="73"/>
-      <c r="E40" s="86"/>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B40" s="109"/>
+      <c r="C40" s="110"/>
+      <c r="D40" s="112"/>
+      <c r="E40" s="75"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="75">
-        <v>1</v>
-      </c>
-      <c r="C41" s="76" t="s">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B41" s="66">
+        <v>1</v>
+      </c>
+      <c r="C41" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="74" t="s">
+      <c r="D41" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="86"/>
+      <c r="E41" s="75"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="77">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B42" s="68">
         <v>2</v>
       </c>
       <c r="C42" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="D42" s="78"/>
-      <c r="E42" s="86"/>
+      <c r="D42" s="102"/>
+      <c r="E42" s="75"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="77">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" s="68">
         <v>3</v>
       </c>
       <c r="C43" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="D43" s="78"/>
-      <c r="E43" s="86"/>
+      <c r="D43" s="102"/>
+      <c r="E43" s="75"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="79">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B44" s="69">
         <v>4</v>
       </c>
-      <c r="C44" s="80" t="s">
+      <c r="C44" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="D44" s="81"/>
-      <c r="E44" s="86"/>
+      <c r="D44" s="113"/>
+      <c r="E44" s="75"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="75">
-        <v>1</v>
-      </c>
-      <c r="C45" s="82" t="s">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B45" s="66">
+        <v>1</v>
+      </c>
+      <c r="C45" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="D45" s="74" t="s">
+      <c r="D45" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="E45" s="86"/>
+      <c r="E45" s="75"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="77">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B46" s="68">
         <v>2</v>
       </c>
       <c r="C46" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="78"/>
-      <c r="E46" s="86"/>
+      <c r="D46" s="102"/>
+      <c r="E46" s="75"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B47" s="77">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B47" s="68">
         <v>3</v>
       </c>
       <c r="C47" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="D47" s="78"/>
-      <c r="E47" s="86"/>
+      <c r="D47" s="102"/>
+      <c r="E47" s="75"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="77">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B48" s="68">
         <v>4</v>
       </c>
       <c r="C48" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="D48" s="78"/>
-      <c r="E48" s="86"/>
+      <c r="D48" s="102"/>
+      <c r="E48" s="75"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B49" s="77">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B49" s="68">
         <v>5</v>
       </c>
       <c r="C49" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="D49" s="78"/>
-      <c r="E49" s="86"/>
+      <c r="D49" s="102"/>
+      <c r="E49" s="75"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B50" s="77">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B50" s="68">
         <v>6</v>
       </c>
       <c r="C50" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="D50" s="78"/>
-      <c r="E50" s="86"/>
+      <c r="D50" s="102"/>
+      <c r="E50" s="75"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="83"/>
-      <c r="C51" s="84" t="s">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B51" s="72"/>
+      <c r="C51" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="85" t="s">
+      <c r="D51" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="86"/>
+      <c r="E51" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E14:E33"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="E2:E9"/>
     <mergeCell ref="D45:D50"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -28147,10 +28124,6 @@
     <mergeCell ref="D41:D44"/>
     <mergeCell ref="B14:B31"/>
     <mergeCell ref="C14:C31"/>
-    <mergeCell ref="E14:E33"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="E2:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>